<commit_message>
add pandas assign to Unit 5
</commit_message>
<xml_diff>
--- a/Unit 5/output/myDFNarrowA.xlsx
+++ b/Unit 5/output/myDFNarrowA.xlsx
@@ -66,6 +66,74 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 

</xml_diff>